<commit_message>
MicroSD card holder has reached end of life
Will need to find a replacement card holder and/or redesign the CPU board to mount the new card holder.
</commit_message>
<xml_diff>
--- a/Hardware_files/OWHL_RevC_parts_list_20160805.xlsx
+++ b/Hardware_files/OWHL_RevC_parts_list_20160805.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arduino\OWHL\Eagle_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arduino\OWHL\Hardware_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6860EC2-1505-4E7D-8139-3EF3B148E722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1770" windowWidth="14360" windowHeight="12080"/>
+    <workbookView xWindow="15970" yWindow="780" windowWidth="22070" windowHeight="18850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RevC_partslist" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,25 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="218">
   <si>
     <t>PCB name</t>
   </si>
@@ -675,12 +689,15 @@
   </si>
   <si>
     <t>36-3000-ND</t>
+  </si>
+  <si>
+    <t>END OF LIFE - will require replacement part and possible board re-design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -715,12 +732,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -785,15 +808,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -804,71 +826,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -879,18 +872,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
@@ -905,326 +896,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1320,52 +991,53 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.499984740745262"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.499984740745262"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.499984740745262"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1410,7 +1082,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="General_parts_list"/>
@@ -1423,9 +1095,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1463,9 +1135,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1500,7 +1172,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1535,7 +1207,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1708,11 +1380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1720,7 +1395,7 @@
     <col min="1" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="20.7265625" customWidth="1"/>
     <col min="4" max="4" width="35.1796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" style="8" customWidth="1"/>
     <col min="8" max="8" width="15.26953125" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" customWidth="1"/>
     <col min="13" max="13" width="10.36328125" customWidth="1"/>
@@ -1728,1361 +1403,1249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="13" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="11">
         <v>1</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="12">
         <v>0.11</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="12">
         <v>0.11</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="17">
+      <c r="O2" s="13">
         <f>G2*I2</f>
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="12">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="12">
         <v>0.1</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="17">
+      <c r="O3" s="13">
         <f t="shared" ref="O3:O26" si="0">G3*I3</f>
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="11">
         <v>4</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="12">
         <v>0.43</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="12">
         <v>0.65</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="12">
         <v>0.45</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="17">
+      <c r="O4" s="13">
         <f t="shared" si="0"/>
         <v>1.72</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>2</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="12">
         <v>0.34</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="12">
         <v>0.7</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="12">
         <v>0.41</v>
       </c>
-      <c r="N5" s="12"/>
-      <c r="O5" s="17">
+      <c r="O5" s="13">
         <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="8">
         <v>1</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" t="s">
         <v>153</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="13">
         <v>0.41</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" t="s">
         <v>185</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="12">
         <v>0.48</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" t="s">
         <v>184</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="12">
         <v>0.48</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="17">
+      <c r="O6" s="13">
         <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="11">
         <v>2</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="12">
         <v>0.1</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="12">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="12">
         <v>0.09</v>
       </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="17">
+      <c r="O7" s="13">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="11">
         <v>2</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="12">
         <v>0.1</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="12">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="12">
         <v>0.1</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="17">
+      <c r="O8" s="13">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+      <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="11">
         <v>4</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="12">
         <v>0.1</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="12">
         <v>0.09</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="12">
         <v>0.1</v>
       </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="17">
+      <c r="O9" s="13">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" t="s">
         <v>160</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="11">
         <v>2</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="12">
         <v>0.1</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="12">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="12">
         <v>0.1</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="17">
+      <c r="O10" s="13">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="11">
         <v>1</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="12">
         <v>1.1100000000000001</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="12">
         <v>1.53</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" t="s">
         <v>70</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <v>1.2</v>
       </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="17">
+      <c r="O11" s="13">
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="11">
         <v>1</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="12">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="12">
         <v>0.505</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="17">
+      <c r="M12" s="12"/>
+      <c r="O12" s="13">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="C13" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="11">
         <v>1</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="12">
         <v>0.1</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="12">
         <v>0.03</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="17">
+      <c r="M13" s="12"/>
+      <c r="O13" s="13">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12" t="s">
+      <c r="C14" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="11">
         <v>6</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" t="s">
         <v>85</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="12">
         <v>0.1</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="12">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="17">
+      <c r="M14" s="12"/>
+      <c r="O14" s="13">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="17">
         <v>1</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="18">
         <v>0.22</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="18">
         <v>0.2</v>
       </c>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M15" s="27">
+      <c r="M15" s="18">
         <v>0.19</v>
       </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="17">
+      <c r="O15" s="13">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" t="s">
         <v>165</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="11">
         <v>1</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" t="s">
         <v>215</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="12">
         <v>0.38</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="12">
         <v>0.37</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" t="s">
         <v>99</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="12">
         <v>0.4</v>
       </c>
-      <c r="N16" s="12"/>
-      <c r="O16" s="17">
+      <c r="O16" s="13">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="11">
         <v>1</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" t="s">
         <v>104</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="12">
         <v>1.7</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" t="s">
         <v>187</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="12">
         <v>2.25</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" t="s">
         <v>105</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="12">
         <v>2.14</v>
       </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="17">
+      <c r="O17" s="13">
         <f t="shared" si="0"/>
         <v>1.7</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>154</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="11">
         <v>2</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="12">
         <v>0.82</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" t="s">
         <v>112</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="12">
         <v>0.75800000000000001</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="L18" t="s">
         <v>113</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="12">
         <v>0.6</v>
       </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="17">
+      <c r="O18" s="13">
         <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="17">
         <v>1</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="18">
         <v>0.54</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K19" s="18">
         <v>0.184</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="L19" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M19" s="27">
+      <c r="M19" s="18">
         <v>0.39</v>
       </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="17">
+      <c r="O19" s="13">
         <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" t="s">
         <v>168</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" t="s">
         <v>212</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="8">
         <v>3</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" t="s">
         <v>121</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="13">
         <v>0.68</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="13">
         <v>0.48</v>
       </c>
-      <c r="L20" s="30"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="17">
+      <c r="M20" s="13"/>
+      <c r="O20" s="13">
         <f t="shared" si="0"/>
         <v>2.04</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
+    <row r="21" spans="1:16" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" t="s">
         <v>168</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="24">
         <v>6</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="25">
         <v>1.33</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="K21" s="42">
+      <c r="K21" s="25">
         <v>1.38</v>
       </c>
-      <c r="L21" s="37" t="s">
+      <c r="L21" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="M21" s="42">
+      <c r="M21" s="25">
         <v>1.54</v>
       </c>
-      <c r="N21" s="37"/>
-      <c r="O21" s="17">
+      <c r="O21" s="13">
         <f t="shared" si="0"/>
         <v>7.98</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" t="s">
         <v>127</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="8">
         <v>1</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" t="s">
         <v>129</v>
       </c>
-      <c r="I22" s="35">
+      <c r="I22" s="13">
         <v>2.0699999999999998</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="13">
         <v>2.2799999999999998</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L22" t="s">
         <v>131</v>
       </c>
-      <c r="M22" s="15">
+      <c r="M22" s="12">
         <v>2.0699999999999998</v>
       </c>
-      <c r="N22" s="30"/>
-      <c r="O22" s="17">
+      <c r="O22" s="13">
         <f t="shared" si="0"/>
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+    <row r="23" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="17">
         <v>1</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="18">
         <v>9.0500000000000007</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K23" s="18">
         <v>10.43</v>
       </c>
-      <c r="L23" s="43" t="s">
+      <c r="L23" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="M23" s="27">
+      <c r="M23" s="18">
         <v>10.43</v>
       </c>
-      <c r="N23" s="24"/>
-      <c r="O23" s="17">
+      <c r="O23" s="13">
         <f t="shared" si="0"/>
         <v>9.0500000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" t="s">
         <v>151</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="11">
         <v>1</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" t="s">
         <v>149</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="12">
         <v>3.47</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" t="s">
         <v>173</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="12">
         <v>3.21</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" t="s">
         <v>172</v>
       </c>
-      <c r="M24" s="15">
+      <c r="M24" s="12">
         <v>3.15</v>
       </c>
-      <c r="N24" s="30"/>
-      <c r="O24" s="17">
+      <c r="O24" s="13">
         <f t="shared" si="0"/>
         <v>3.47</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
+      <c r="P24" s="32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" t="s">
         <v>142</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="10">
         <v>3000</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="11">
         <v>1</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H25" t="s">
         <v>216</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="12">
         <v>0.52</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J25" t="s">
         <v>143</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="12">
         <v>0.3</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" t="s">
         <v>144</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="12">
         <v>0.54</v>
       </c>
-      <c r="N25" s="12"/>
-      <c r="O25" s="17">
+      <c r="O25" s="13">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" t="s">
         <v>147</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="11">
         <v>1</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="H26" t="s">
         <v>169</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="12">
         <v>13.82</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" t="s">
         <v>170</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="12">
         <v>22.04</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="L26" t="s">
         <v>171</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M26" s="12">
         <v>21.82</v>
       </c>
-      <c r="N26" s="12"/>
-      <c r="O26" s="17">
+      <c r="O26" s="13">
         <f t="shared" si="0"/>
         <v>13.82</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N28" t="s">
         <v>210</v>
       </c>
-      <c r="O28" s="17">
+      <c r="O28" s="13">
         <f>SUM(O2:O26)</f>
         <v>50.17</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C11:C13 A1:C5 C15:C20 A22:C26 E6 C6:C9 A6:B20">
-    <cfRule type="containsText" dxfId="54" priority="88" operator="containsText" text="alternate">
+  <conditionalFormatting sqref="A1:C20">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="alternate">
       <formula>NOT(ISERROR(SEARCH("alternate",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="89" operator="containsText" text="main">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="main">
       <formula>NOT(ISERROR(SEARCH("main",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C13 A1:C5 C15:C23 A24:C26 E6 C6:C9 A6:B23">
-    <cfRule type="cellIs" dxfId="52" priority="87" operator="equal">
+  <conditionalFormatting sqref="A1:C26">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="45" priority="67" operator="containsText" text="alternate">
+  <conditionalFormatting sqref="A22:C26">
+    <cfRule type="containsText" dxfId="15" priority="88" operator="containsText" text="alternate">
+      <formula>NOT(ISERROR(SEARCH("alternate",A22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="89" operator="containsText" text="main">
+      <formula>NOT(ISERROR(SEARCH("main",A22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="alternate">
+      <formula>NOT(ISERROR(SEARCH("alternate",B21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="main">
+      <formula>NOT(ISERROR(SEARCH("main",B21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E6">
+    <cfRule type="cellIs" dxfId="11" priority="45" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="46" operator="containsText" text="alternate">
+      <formula>NOT(ISERROR(SEARCH("alternate",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="47" operator="containsText" text="main">
+      <formula>NOT(ISERROR(SEARCH("main",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E14">
+    <cfRule type="cellIs" dxfId="8" priority="60" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="61" operator="containsText" text="alternate">
       <formula>NOT(ISERROR(SEARCH("alternate",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="68" operator="containsText" text="main">
+    <cfRule type="containsText" dxfId="6" priority="62" operator="containsText" text="main">
       <formula>NOT(ISERROR(SEARCH("main",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="43" priority="66" operator="equal">
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="42" priority="64" operator="containsText" text="alternate">
-      <formula>NOT(ISERROR(SEARCH("alternate",E13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="65" operator="containsText" text="main">
-      <formula>NOT(ISERROR(SEARCH("main",E13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="40" priority="63" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="39" priority="61" operator="containsText" text="alternate">
-      <formula>NOT(ISERROR(SEARCH("alternate",E14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="62" operator="containsText" text="main">
-      <formula>NOT(ISERROR(SEARCH("main",E14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="37" priority="60" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="34" priority="52" operator="containsText" text="alternate">
+    <cfRule type="containsText" dxfId="4" priority="52" operator="containsText" text="alternate">
       <formula>NOT(ISERROR(SEARCH("alternate",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="53" operator="containsText" text="main">
+    <cfRule type="containsText" dxfId="3" priority="53" operator="containsText" text="main">
       <formula>NOT(ISERROR(SEARCH("main",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="32" priority="51" operator="equal">
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="2" priority="30" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="30" priority="46" operator="containsText" text="alternate">
-      <formula>NOT(ISERROR(SEARCH("alternate",E5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="47" operator="containsText" text="main">
-      <formula>NOT(ISERROR(SEARCH("main",E5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="28" priority="45" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="25" priority="40" operator="containsText" text="alternate">
-      <formula>NOT(ISERROR(SEARCH("alternate",C10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="41" operator="containsText" text="main">
-      <formula>NOT(ISERROR(SEARCH("main",C10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="containsText" dxfId="21" priority="31" operator="containsText" text="alternate">
+    <cfRule type="containsText" dxfId="1" priority="31" operator="containsText" text="alternate">
       <formula>NOT(ISERROR(SEARCH("alternate",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="32" operator="containsText" text="main">
+    <cfRule type="containsText" dxfId="0" priority="32" operator="containsText" text="main">
       <formula>NOT(ISERROR(SEARCH("main",E22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="19" priority="30" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="alternate">
-      <formula>NOT(ISERROR(SEARCH("alternate",C14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="main">
-      <formula>NOT(ISERROR(SEARCH("main",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="alternate">
-      <formula>NOT(ISERROR(SEARCH("alternate",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="main">
-      <formula>NOT(ISERROR(SEARCH("main",B21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ102V/P1.0KACT-ND/42833"/>
-    <hyperlink ref="J8" r:id="rId2" tooltip="65T8778" display="http://www.newark.com/panasonic/erj-6geyj102v/resistor-thick-film-0805-1kohm/dp/65T8778"/>
-    <hyperlink ref="J4" r:id="rId3" tooltip="84R9733" display="http://www.newark.com/taiyo-yuden/lmk212sd104kg-t/capacitor-ceramic-0-1uf-10v-0805/dp/84R9733"/>
-    <hyperlink ref="H7" r:id="rId4" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ511V/P510ACT-ND/90030"/>
-    <hyperlink ref="J7" r:id="rId5" tooltip="65T8831" display="http://www.newark.com/panasonic/erj-6geyj511v/resistor-chip-thick-film-510-ohm/dp/65T8831"/>
-    <hyperlink ref="J13" r:id="rId6" tooltip="28C6963" display="http://www.newark.com/jst-japan-solderless-terminals/phr-2/wire-to-board-connector-housing/dp/28C6963"/>
-    <hyperlink ref="J14" r:id="rId7" tooltip="28C6968" display="http://www.newark.com/jst-japan-solderless-terminals/sph-002t-p0-5s/contact-pin-30-24awg-crimp/dp/28C6968"/>
-    <hyperlink ref="J5" r:id="rId8" tooltip="53W3651" display="http://www.newark.com/panasonic/eee-fc1v1r0r/capacitor-alum-elec-1uf-35v-20/dp/53W3651"/>
-    <hyperlink ref="L9" r:id="rId9" tooltip="Click to view additional information on this product." display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-6GEYJ103V/?qs=sGAEpiMZZMu61qfTUdNhGzRxdwze5h8ZVHioc%2fD1YKQ%3d"/>
-    <hyperlink ref="J9" r:id="rId10" tooltip="67T1248" display="http://www.newark.com/panasonic/erj-6geyj103v/resistor-10kohm-125mw-5/dp/67T1248"/>
-    <hyperlink ref="H9" r:id="rId11" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ103V/P10KACT-ND/43118"/>
-    <hyperlink ref="H10" r:id="rId12" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ104V/P100KACT-ND/692"/>
-    <hyperlink ref="J10" r:id="rId13" tooltip="65T8779" display="http://www.newark.com/panasonic/erj-6geyj104v/resistor-chip-thick-film-100-kohm/dp/65T8779"/>
-    <hyperlink ref="J20" r:id="rId14" tooltip="BG095-06-A-N-D" display="http://www.newark.com/global-connector-technology/bg095-06-a-n-d/board-board-connector-socket-6way/dp/67R8589"/>
-    <hyperlink ref="L23" r:id="rId15" tooltip="Click to view additional information on this product." display="http://www.mouser.com/ProductDetail/Maxim-Integrated/DS3231SN/?qs=sGAEpiMZZMuuBt6TL7D%2f6MqiKtjHXkRT"/>
-    <hyperlink ref="J16" r:id="rId16" tooltip="84R5176" display="http://www.newark.com/microchip/mcp1700t-3002e-tt/ic-ldo-volt-reg-3v-0-25a-sot-23/dp/84R5176"/>
+    <hyperlink ref="H8" r:id="rId1" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ102V/P1.0KACT-ND/42833" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J8" r:id="rId2" tooltip="65T8778" display="http://www.newark.com/panasonic/erj-6geyj102v/resistor-thick-film-0805-1kohm/dp/65T8778" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" tooltip="84R9733" display="http://www.newark.com/taiyo-yuden/lmk212sd104kg-t/capacitor-ceramic-0-1uf-10v-0805/dp/84R9733" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H7" r:id="rId4" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ511V/P510ACT-ND/90030" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J7" r:id="rId5" tooltip="65T8831" display="http://www.newark.com/panasonic/erj-6geyj511v/resistor-chip-thick-film-510-ohm/dp/65T8831" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J13" r:id="rId6" tooltip="28C6963" display="http://www.newark.com/jst-japan-solderless-terminals/phr-2/wire-to-board-connector-housing/dp/28C6963" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J14" r:id="rId7" tooltip="28C6968" display="http://www.newark.com/jst-japan-solderless-terminals/sph-002t-p0-5s/contact-pin-30-24awg-crimp/dp/28C6968" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J5" r:id="rId8" tooltip="53W3651" display="http://www.newark.com/panasonic/eee-fc1v1r0r/capacitor-alum-elec-1uf-35v-20/dp/53W3651" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L9" r:id="rId9" tooltip="Click to view additional information on this product." display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-6GEYJ103V/?qs=sGAEpiMZZMu61qfTUdNhGzRxdwze5h8ZVHioc%2fD1YKQ%3d" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J9" r:id="rId10" tooltip="67T1248" display="http://www.newark.com/panasonic/erj-6geyj103v/resistor-10kohm-125mw-5/dp/67T1248" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H9" r:id="rId11" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ103V/P10KACT-ND/43118" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H10" r:id="rId12" display="http://www.digikey.com/product-detail/en/ERJ-6GEYJ104V/P100KACT-ND/692" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J10" r:id="rId13" tooltip="65T8779" display="http://www.newark.com/panasonic/erj-6geyj104v/resistor-chip-thick-film-100-kohm/dp/65T8779" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J20" r:id="rId14" tooltip="BG095-06-A-N-D" display="http://www.newark.com/global-connector-technology/bg095-06-a-n-d/board-board-connector-socket-6way/dp/67R8589" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L23" r:id="rId15" tooltip="Click to view additional information on this product." display="http://www.mouser.com/ProductDetail/Maxim-Integrated/DS3231SN/?qs=sGAEpiMZZMuuBt6TL7D%2f6MqiKtjHXkRT" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J16" r:id="rId16" tooltip="84R5176" display="http://www.newark.com/microchip/mcp1700t-3002e-tt/ic-ldo-volt-reg-3v-0-25a-sot-23/dp/84R5176" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup scale="54" orientation="landscape" r:id="rId17"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -3110,59 +2673,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C21</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="92" operator="containsText" text="alternate" id="{77C11002-3990-4788-9961-B574A2599F86}">
-            <xm:f>NOT(ISERROR(SEARCH("alternate",'C:\Miller_projects\Electronics\OWHL\[PCB_parts_list.xlsx]General_parts_list'!#REF!)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="93" operator="containsText" text="main" id="{3AE3FCCC-5E5B-4B32-9DF5-BD9E322FC1AE}">
-            <xm:f>NOT(ISERROR(SEARCH("main",'C:\Miller_projects\Electronics\OWHL\[PCB_parts_list.xlsx]General_parts_list'!#REF!)))</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="6" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B21</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="94" operator="containsText" text="alternate" id="{E5DAD2AC-A3B7-4F1A-BD94-16FAE4275163}">
-            <xm:f>NOT(ISERROR(SEARCH("alternate",'C:\Miller_projects\Electronics\OWHL\[PCB_parts_list.xlsx]General_parts_list'!#REF!)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="95" operator="containsText" text="main" id="{612A066B-6042-4FFD-821E-B83C728A6192}">
-            <xm:f>NOT(ISERROR(SEARCH("main",'C:\Miller_projects\Electronics\OWHL\[PCB_parts_list.xlsx]General_parts_list'!#REF!)))</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="6" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A21</xm:sqref>
+          <xm:sqref>A21:C21</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3171,7 +2682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -3181,21 +2692,21 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.08984375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="29.08984375" style="8" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3206,7 +2717,7 @@
       <c r="B2" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -3220,7 +2731,7 @@
       <c r="B3" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -3234,7 +2745,7 @@
       <c r="B4" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>3</v>
       </c>
       <c r="D4" t="s">
@@ -3248,7 +2759,7 @@
       <c r="B5" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>4</v>
       </c>
       <c r="D5" t="s">
@@ -3262,7 +2773,7 @@
       <c r="B6" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>5</v>
       </c>
       <c r="D6" t="s">
@@ -3276,7 +2787,7 @@
       <c r="B7" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>6</v>
       </c>
       <c r="D7" t="s">
@@ -3290,7 +2801,7 @@
       <c r="B8" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
@@ -3304,7 +2815,7 @@
       <c r="B9" t="s">
         <v>196</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>2</v>
       </c>
       <c r="D9" t="s">
@@ -3318,7 +2829,7 @@
       <c r="B10" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>3</v>
       </c>
       <c r="D10" t="s">
@@ -3332,7 +2843,7 @@
       <c r="B11" t="s">
         <v>196</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>4</v>
       </c>
       <c r="D11" t="s">
@@ -3346,7 +2857,7 @@
       <c r="B12" t="s">
         <v>196</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>5</v>
       </c>
       <c r="D12" t="s">
@@ -3360,7 +2871,7 @@
       <c r="B13" t="s">
         <v>196</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>6</v>
       </c>
       <c r="D13" t="s">
@@ -3374,7 +2885,7 @@
       <c r="B14" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>1</v>
       </c>
       <c r="D14" t="s">
@@ -3388,7 +2899,7 @@
       <c r="B15" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>2</v>
       </c>
       <c r="D15" t="s">
@@ -3402,7 +2913,7 @@
       <c r="B16" t="s">
         <v>200</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>3</v>
       </c>
       <c r="D16" t="s">
@@ -3416,7 +2927,7 @@
       <c r="B17" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>4</v>
       </c>
       <c r="D17" t="s">
@@ -3430,7 +2941,7 @@
       <c r="B18" t="s">
         <v>200</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>5</v>
       </c>
       <c r="D18" t="s">
@@ -3444,7 +2955,7 @@
       <c r="B19" t="s">
         <v>200</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>6</v>
       </c>
       <c r="D19" t="s">
@@ -3458,7 +2969,7 @@
       <c r="B20" t="s">
         <v>204</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>1</v>
       </c>
       <c r="D20" t="s">
@@ -3472,7 +2983,7 @@
       <c r="B21" t="s">
         <v>204</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>2</v>
       </c>
       <c r="D21" t="s">
@@ -3486,7 +2997,7 @@
       <c r="B22" t="s">
         <v>204</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>3</v>
       </c>
       <c r="D22" t="s">
@@ -3500,7 +3011,7 @@
       <c r="B23" t="s">
         <v>204</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>4</v>
       </c>
       <c r="D23" t="s">
@@ -3514,7 +3025,7 @@
       <c r="B24" t="s">
         <v>204</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>5</v>
       </c>
       <c r="D24" t="s">
@@ -3528,7 +3039,7 @@
       <c r="B25" t="s">
         <v>204</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>6</v>
       </c>
       <c r="D25" t="s">
@@ -3542,7 +3053,7 @@
       <c r="B26" t="s">
         <v>196</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <v>1</v>
       </c>
       <c r="D26" t="s">
@@ -3556,7 +3067,7 @@
       <c r="B27" t="s">
         <v>196</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>2</v>
       </c>
       <c r="D27" t="s">
@@ -3570,7 +3081,7 @@
       <c r="B28" t="s">
         <v>196</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>3</v>
       </c>
       <c r="D28" t="s">
@@ -3584,7 +3095,7 @@
       <c r="B29" t="s">
         <v>196</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>4</v>
       </c>
       <c r="D29" t="s">
@@ -3598,7 +3109,7 @@
       <c r="B30" t="s">
         <v>196</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>5</v>
       </c>
       <c r="D30" t="s">
@@ -3612,7 +3123,7 @@
       <c r="B31" t="s">
         <v>196</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <v>6</v>
       </c>
       <c r="D31" t="s">
@@ -3626,7 +3137,7 @@
       <c r="B32" t="s">
         <v>200</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" t="s">
@@ -3640,7 +3151,7 @@
       <c r="B33" t="s">
         <v>200</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <v>2</v>
       </c>
       <c r="D33" t="s">
@@ -3654,7 +3165,7 @@
       <c r="B34" t="s">
         <v>200</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <v>3</v>
       </c>
       <c r="D34" t="s">
@@ -3668,7 +3179,7 @@
       <c r="B35" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <v>4</v>
       </c>
       <c r="D35" t="s">
@@ -3682,7 +3193,7 @@
       <c r="B36" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <v>5</v>
       </c>
       <c r="D36" t="s">
@@ -3696,7 +3207,7 @@
       <c r="B37" t="s">
         <v>200</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <v>6</v>
       </c>
       <c r="D37" t="s">
@@ -3710,7 +3221,7 @@
       <c r="B38" t="s">
         <v>204</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <v>1</v>
       </c>
       <c r="D38" t="s">
@@ -3724,7 +3235,7 @@
       <c r="B39" t="s">
         <v>204</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <v>2</v>
       </c>
       <c r="D39" t="s">
@@ -3738,7 +3249,7 @@
       <c r="B40" t="s">
         <v>204</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <v>3</v>
       </c>
       <c r="D40" t="s">
@@ -3752,7 +3263,7 @@
       <c r="B41" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8">
         <v>4</v>
       </c>
       <c r="D41" t="s">
@@ -3766,7 +3277,7 @@
       <c r="B42" t="s">
         <v>204</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <v>5</v>
       </c>
       <c r="D42" t="s">
@@ -3780,7 +3291,7 @@
       <c r="B43" t="s">
         <v>204</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8">
         <v>6</v>
       </c>
       <c r="D43" t="s">
@@ -3794,7 +3305,7 @@
       <c r="B44" t="s">
         <v>196</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" t="s">
@@ -3808,7 +3319,7 @@
       <c r="B45" t="s">
         <v>196</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8">
         <v>2</v>
       </c>
       <c r="D45" t="s">
@@ -3822,7 +3333,7 @@
       <c r="B46" t="s">
         <v>196</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="8">
         <v>3</v>
       </c>
       <c r="D46" t="s">
@@ -3836,7 +3347,7 @@
       <c r="B47" t="s">
         <v>196</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8">
         <v>4</v>
       </c>
       <c r="D47" t="s">
@@ -3850,7 +3361,7 @@
       <c r="B48" t="s">
         <v>196</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8">
         <v>5</v>
       </c>
       <c r="D48" t="s">
@@ -3864,7 +3375,7 @@
       <c r="B49" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="8">
         <v>6</v>
       </c>
       <c r="D49" t="s">
@@ -3878,7 +3389,7 @@
       <c r="B50" t="s">
         <v>200</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8">
         <v>1</v>
       </c>
       <c r="D50" t="s">
@@ -3892,7 +3403,7 @@
       <c r="B51" t="s">
         <v>200</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8">
         <v>2</v>
       </c>
       <c r="D51" t="s">
@@ -3906,7 +3417,7 @@
       <c r="B52" t="s">
         <v>200</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="8">
         <v>3</v>
       </c>
       <c r="D52" t="s">
@@ -3920,7 +3431,7 @@
       <c r="B53" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="8">
         <v>4</v>
       </c>
       <c r="D53" t="s">
@@ -3934,7 +3445,7 @@
       <c r="B54" t="s">
         <v>200</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="8">
         <v>5</v>
       </c>
       <c r="D54" t="s">
@@ -3948,7 +3459,7 @@
       <c r="B55" t="s">
         <v>200</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C55" s="8">
         <v>6</v>
       </c>
       <c r="D55" t="s">
@@ -3962,7 +3473,7 @@
       <c r="B56" t="s">
         <v>204</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8">
         <v>1</v>
       </c>
       <c r="D56" t="s">
@@ -3976,7 +3487,7 @@
       <c r="B57" t="s">
         <v>204</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="8">
         <v>2</v>
       </c>
       <c r="D57" t="s">
@@ -3990,7 +3501,7 @@
       <c r="B58" t="s">
         <v>204</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="8">
         <v>3</v>
       </c>
       <c r="D58" t="s">
@@ -4004,7 +3515,7 @@
       <c r="B59" t="s">
         <v>204</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8">
         <v>4</v>
       </c>
       <c r="D59" t="s">
@@ -4018,7 +3529,7 @@
       <c r="B60" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8">
         <v>5</v>
       </c>
       <c r="D60" t="s">
@@ -4032,7 +3543,7 @@
       <c r="B61" t="s">
         <v>204</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8">
         <v>6</v>
       </c>
       <c r="D61" t="s">
@@ -4045,7 +3556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>